<commit_message>
Update PM21 Tidsregistrering for Lukas.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM21 Tidsregistrering for Lukas.xlsx
+++ b/08 Project Management/Tidsregistrering/PM21 Tidsregistrering for Lukas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Skrivebord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Documents\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61EF5623-0EE8-4DDE-BE0D-B604184B349E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{61EF5623-0EE8-4DDE-BE0D-B604184B349E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0DABC032-D979-448A-A814-A43A2413B2A5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="Roller">'Ark2'!$B$3:$B$31</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Stakeholders</t>
+  </si>
+  <si>
+    <t>Review UC12</t>
+  </si>
+  <si>
+    <t>Review + Edit DOM12</t>
   </si>
 </sst>
 </file>
@@ -175,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +227,13 @@
     <font>
       <b/>
       <sz val="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -316,7 +329,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -331,9 +344,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,35 +351,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -452,7 +461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -748,52 +757,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="53.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="31" style="17" customWidth="1"/>
-    <col min="6" max="6" width="31" style="22" customWidth="1"/>
+    <col min="1" max="2" width="53.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="31" style="13" customWidth="1"/>
+    <col min="6" max="6" width="31" style="23" customWidth="1"/>
     <col min="7" max="7" width="37.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="37.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.6">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" ht="19.899999999999999">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -803,23 +812,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.899999999999999">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="20">
         <v>43895</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>0.625</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>0.64583333333333337</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="23">
         <v>15</v>
       </c>
       <c r="G3" s="5">
@@ -831,23 +840,23 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.899999999999999">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="20">
         <v>43895</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="23">
         <v>15</v>
       </c>
       <c r="G4" s="5">
@@ -859,396 +868,335 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.899999999999999">
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="21"/>
+    <row r="5" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="21">
+        <v>43896</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F5" s="23">
+        <v>30</v>
+      </c>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="H5" s="1">
         <f>SUM(G$3:G5)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.899999999999999">
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="21">
+        <v>43896</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.5625</v>
+      </c>
+      <c r="F6" s="23">
+        <v>60</v>
+      </c>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14583333333333331</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(G$3:G6)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19.899999999999999">
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19.899999999999999">
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19.899999999999999">
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="19.899999999999999">
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="19.899999999999999">
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19.899999999999999">
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19.899999999999999">
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19.899999999999999">
-      <c r="C14" s="15"/>
-      <c r="F14" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19.899999999999999">
-      <c r="C15" s="15"/>
-      <c r="F15" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19.899999999999999">
-      <c r="C16" s="15"/>
-      <c r="F16" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="19.899999999999999">
-      <c r="C17" s="15"/>
-      <c r="F17" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="19.899999999999999">
-      <c r="C18" s="15"/>
-      <c r="F18" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="19.899999999999999">
-      <c r="C19" s="15"/>
-      <c r="F19" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="19.899999999999999">
-      <c r="C20" s="15"/>
-      <c r="F20" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="19.899999999999999">
-      <c r="C21" s="15"/>
-      <c r="F21" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" ht="19.899999999999999">
-      <c r="C22" s="15"/>
-      <c r="F22" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="19.899999999999999">
-      <c r="C23" s="15"/>
-      <c r="F23" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="19.899999999999999">
-      <c r="C24" s="15"/>
-      <c r="F24" s="21"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="19.899999999999999">
-      <c r="C25" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="19.899999999999999">
-      <c r="C26" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="19.899999999999999">
-      <c r="C27" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" ht="19.899999999999999">
-      <c r="C28" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G28" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="19.899999999999999">
-      <c r="C29" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G29" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" ht="19.899999999999999">
-      <c r="C30" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G30" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" ht="19.899999999999999">
-      <c r="C31" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G31" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="19.899999999999999">
-      <c r="C32" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G32" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="3:3">
-      <c r="C34" s="15"/>
-    </row>
-    <row r="35" spans="3:3">
-      <c r="C35" s="15"/>
-    </row>
-    <row r="36" spans="3:3">
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="3:3">
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="3:3">
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="3:3">
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="3:3">
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="3:3">
-      <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="3:3">
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="3:3">
-      <c r="C43" s="15"/>
-    </row>
-    <row r="44" spans="3:3">
-      <c r="C44" s="15"/>
-    </row>
-    <row r="45" spans="3:3">
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="3:3">
-      <c r="C47" s="15"/>
+        <v>0.22916666666666663</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1258,11 +1206,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{BFDCDBAC-12D7-4CE8-B28E-3FB0550AF167}">
       <formula1>Roller</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{EAF4FEC8-302E-4BC5-B847-882BBAE51A3C}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4 C7:C1048576" xr:uid="{EAF4FEC8-302E-4BC5-B847-882BBAE51A3C}">
       <formula1>43881</formula1>
       <formula2>43908</formula2>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{AAB748DE-A874-498A-B6D5-9F9C72DDE532}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D4 D7:D1048576" xr:uid="{AAB748DE-A874-498A-B6D5-9F9C72DDE532}">
       <formula1>0.333333333333333</formula1>
       <formula2>0.708333333333333</formula2>
     </dataValidation>
@@ -1281,21 +1229,21 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1303,7 +1251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1311,7 +1259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1319,7 +1267,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1327,7 +1275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1335,7 +1283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1343,7 +1291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1351,7 +1299,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1359,7 +1307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1367,7 +1315,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1375,7 +1323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1383,7 +1331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1391,7 +1339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1399,7 +1347,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1407,7 +1355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1415,7 +1363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1423,7 +1371,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1431,7 +1379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1439,7 +1387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1447,7 +1395,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1455,7 +1403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1463,7 +1411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1471,7 +1419,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1479,7 +1427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1487,7 +1435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1495,7 +1443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1503,7 +1451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1511,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1519,7 +1467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1527,7 +1475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>

</xml_diff>